<commit_message>
working pdf and excel report
</commit_message>
<xml_diff>
--- a/outputs/monthly_report.xlsx
+++ b/outputs/monthly_report.xlsx
@@ -564,7 +564,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Income</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Income</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,36 +634,26 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2000</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-195</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Transport</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
         <v>-22.75</v>
       </c>
     </row>

</xml_diff>